<commit_message>
Added the ability to data scraping the website "Eldorado".
</commit_message>
<xml_diff>
--- a/comfy_data.xlsx
+++ b/comfy_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="244">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="240">
   <x:si>
     <x:t>Назва</x:t>
   </x:si>
@@ -397,18 +397,18 @@
     <x:t>https://comfy.ua/ua/smartfon-samsung-galaxy-a04-4-64gb-black-sm-a045fzkgsek.html</x:t>
   </x:si>
   <x:si>
+    <x:t>Смартфон Samsung Galaxy A04s 3/32Gb Green (SM-A047FZGUSEK)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://comfy.ua/ua/smartfon-samsung-galaxy-a04s-3-32gb-green-sm-a047fzgusek.html</x:t>
+  </x:si>
+  <x:si>
     <x:t>Смартфон Samsung Galaxy A04s 3/32Gb Copper (SM-A047FZCUSEK)</x:t>
   </x:si>
   <x:si>
     <x:t>https://comfy.ua/ua/smartfon-samsung-galaxy-a04s-3-32gb-copper-sm-a047fzcusek.html</x:t>
   </x:si>
   <x:si>
-    <x:t>Смартфон Samsung Galaxy A04s 3/32Gb Green (SM-A047FZGUSEK)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://comfy.ua/ua/smartfon-samsung-galaxy-a04s-3-32gb-green-sm-a047fzgusek.html</x:t>
-  </x:si>
-  <x:si>
     <x:t>Смартфон Samsung Galaxy A04s 3/32Gb Black (SM-A047FZKUSEK)</x:t>
   </x:si>
   <x:si>
@@ -421,24 +421,24 @@
     <x:t>https://comfy.ua/ua/smartfon-samsung-galaxy-a13-3-32gb-white-sm-a135fzwusek.html</x:t>
   </x:si>
   <x:si>
+    <x:t>Смартфон Samsung Galaxy A04s 4/64Gb Green (SM-A047FZGVSEK)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://comfy.ua/ua/smartfon-samsung-galaxy-a04s-4-64gb-green-sm-a047fzgvsek.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Смартфон Samsung Galaxy A04s 4/64Gb Black (SM-A047FZKVSEK)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://comfy.ua/ua/smartfon-samsung-galaxy-a04s-4-64gb-black-sm-a047fzkvsek.html</x:t>
+  </x:si>
+  <x:si>
     <x:t>Смартфон Samsung Galaxy A04s 4/64Gb Copper (SM-A047FZCVSEK)</x:t>
   </x:si>
   <x:si>
     <x:t>https://comfy.ua/ua/smartfon-samsung-galaxy-a04s-4-64gb-copper-sm-a047fzcvsek.html</x:t>
   </x:si>
   <x:si>
-    <x:t>Смартфон Samsung Galaxy A04s 4/64Gb Black (SM-A047FZKVSEK)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://comfy.ua/ua/smartfon-samsung-galaxy-a04s-4-64gb-black-sm-a047fzkvsek.html</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Смартфон Samsung Galaxy A04s 4/64Gb Green (SM-A047FZGVSEK)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://comfy.ua/ua/smartfon-samsung-galaxy-a04s-4-64gb-green-sm-a047fzgvsek.html</x:t>
-  </x:si>
-  <x:si>
     <x:t>Смартфон Samsung Galaxy A13 4/64Gb White (SM-A135FZWVSEK)</x:t>
   </x:si>
   <x:si>
@@ -451,24 +451,24 @@
     <x:t>https://comfy.ua/ua/smartfon-samsung-galaxy-m13-4-128gb-light-blue-sm-m135flbgsek.html</x:t>
   </x:si>
   <x:si>
+    <x:t>Смартфон Samsung Galaxy A23 4/64Gb Orange (SM-A235FZOUSEK)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://comfy.ua/ua/smartfon-samsung-galaxy-a23-4-64gb-orange-sm-a235fzousek.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Смартфон Samsung Galaxy A23 4/64Gb Black (SM-A235FZKUSEK)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://comfy.ua/ua/smartfon-samsung-galaxy-a23-4-64gb-black-sm-a235fzkusek.html</x:t>
+  </x:si>
+  <x:si>
     <x:t>Смартфон Samsung Galaxy A23 4/64Gb White (SM-A235FZWUSEK)</x:t>
   </x:si>
   <x:si>
     <x:t>https://comfy.ua/ua/smartfon-samsung-galaxy-a23-4-64gb-white-sm-a235fzwusek.html</x:t>
   </x:si>
   <x:si>
-    <x:t>Смартфон Samsung Galaxy A23 4/64Gb Orange (SM-A235FZOUSEK)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://comfy.ua/ua/smartfon-samsung-galaxy-a23-4-64gb-orange-sm-a235fzousek.html</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Смартфон Samsung Galaxy A23 4/64Gb Black (SM-A235FZKUSEK)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://comfy.ua/ua/smartfon-samsung-galaxy-a23-4-64gb-black-sm-a235fzkusek.html</x:t>
-  </x:si>
-  <x:si>
     <x:t>Смартфон Samsung Galaxy A23 6/128Gb White (SM-A235FZWKSEK)</x:t>
   </x:si>
   <x:si>
@@ -529,18 +529,18 @@
     <x:t>https://comfy.ua/ua/smartfon-samsung-galaxy-m53-5g-6-128gb-brown-sm-m536bzndsek.html</x:t>
   </x:si>
   <x:si>
+    <x:t>Смартфон Samsung Galaxy A73 5G 6/128Gb White (SM-A736BZWDSEK)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://comfy.ua/ua/smartfon-samsung-galaxy-a73-5g-6-128gb-white-sm-a736bzwdsek.html</x:t>
+  </x:si>
+  <x:si>
     <x:t>Смартфон Samsung Galaxy A73 5G 6/128Gb Light Green (SM-A736BLGDSEK)</x:t>
   </x:si>
   <x:si>
     <x:t>https://comfy.ua/ua/smartfon-samsung-galaxy-a73-5g-6-128gb-light-green-sm-a736blgdsek.html</x:t>
   </x:si>
   <x:si>
-    <x:t>Смартфон Samsung Galaxy A73 5G 6/128Gb White (SM-A736BZWDSEK)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://comfy.ua/ua/smartfon-samsung-galaxy-a73-5g-6-128gb-white-sm-a736bzwdsek.html</x:t>
-  </x:si>
-  <x:si>
     <x:t>Смартфон Samsung Galaxy A73 5G 8/256Gb White (SM-A736BZWHSEK)</x:t>
   </x:si>
   <x:si>
@@ -553,78 +553,72 @@
     <x:t>https://comfy.ua/ua/smartfon-samsung-galaxy-s21fe-6-128gb-white-sm-g990bzwfsek.html</x:t>
   </x:si>
   <x:si>
+    <x:t>Смартфон Samsung Galaxy S21FE 8/256Gb White (SM-G990BZWWSEK)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://comfy.ua/ua/smartfon-samsung-galaxy-s21fe-8-256gb-white-sm-g990bzwwsek.html</x:t>
+  </x:si>
+  <x:si>
     <x:t>Смартфон Samsung Galaxy S21FE 8/256Gb Light Violet (SM-G990BLVWSEK)</x:t>
   </x:si>
   <x:si>
     <x:t>https://comfy.ua/ua/smartfon-samsung-galaxy-s21fe-8-256gb-light-violet-sm-g990blvwsek.html</x:t>
   </x:si>
   <x:si>
-    <x:t>Смартфон Samsung Galaxy S21FE 8/256Gb White (SM-G990BZWWSEK)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://comfy.ua/ua/smartfon-samsung-galaxy-s21fe-8-256gb-white-sm-g990bzwwsek.html</x:t>
-  </x:si>
-  <x:si>
     <x:t>Смартфон Samsung Galaxy S21FE 8/256Gb Light Green (SM-G990BLGWSEK)</x:t>
   </x:si>
   <x:si>
     <x:t>https://comfy.ua/ua/smartfon-samsung-galaxy-s21fe-8-256gb-light-green-sm-g990blgwsek.html</x:t>
   </x:si>
   <x:si>
+    <x:t>Смартфон Samsung Galaxy S22 8/128Gb Pink (SM-S901BIDDSEK)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://comfy.ua/ua/smartfon-samsung-galaxy-s22-8-128gb-pink-sm-s901biddsek.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Смартфон Samsung Galaxy S22 8/128Gb Green (SM-S901BZGDSEK)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://comfy.ua/ua/smartfon-samsung-galaxy-s22-8-128gb-green-sm-s901bzgdsek.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Смартфон Samsung Galaxy S22 8/128Gb Phantom Black (SM-S901BZKDSEK)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://comfy.ua/ua/smartfon-samsung-galaxy-s22-8-128gb-phantom-black-sm-s901bzkdsek.html</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Смартфон Samsung Galaxy S22 8/128Gb Phantom White (SM-S901BZWDSEK)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://comfy.ua/ua/smartfon-samsung-galaxy-s22-8-128gb-phantom-white-sm-s901bzwdsek.html</x:t>
+  </x:si>
+  <x:si>
     <x:t>Смартфон Samsung Galaxy S22 8/128Gb Light Violet (SM-S901BLVDSEK)</x:t>
   </x:si>
   <x:si>
     <x:t>https://comfy.ua/ua/smartfon-samsung-galaxy-s22-8-128gb-light-violet-sm-s901blvdsek.html</x:t>
   </x:si>
   <x:si>
-    <x:t>Смартфон Samsung Galaxy S22 8/128Gb Pink (SM-S901BIDDSEK)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://comfy.ua/ua/smartfon-samsung-galaxy-s22-8-128gb-pink-sm-s901biddsek.html</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Смартфон Samsung Galaxy S22 8/128Gb Green (SM-S901BZGDSEK)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://comfy.ua/ua/smartfon-samsung-galaxy-s22-8-128gb-green-sm-s901bzgdsek.html</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Смартфон Samsung Galaxy S22 8/128Gb Phantom Black (SM-S901BZKDSEK)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://comfy.ua/ua/smartfon-samsung-galaxy-s22-8-128gb-phantom-black-sm-s901bzkdsek.html</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Смартфон Samsung Galaxy S22 8/128Gb Phantom White (SM-S901BZWDSEK)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://comfy.ua/ua/smartfon-samsung-galaxy-s22-8-128gb-phantom-white-sm-s901bzwdsek.html</x:t>
-  </x:si>
-  <x:si>
     <x:t>Смартфон Samsung Galaxy S22 8/256Gb Pink (SM-S901BIDGSEK)</x:t>
   </x:si>
   <x:si>
     <x:t>https://comfy.ua/ua/smartfon-samsung-galaxy-s22-8-256gb-pink-sm-s901bidgsek.html</x:t>
   </x:si>
   <x:si>
+    <x:t>Смартфон Samsung Galaxy S22 8/256Gb Phantom White (SM-S901BZWGSEK)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://comfy.ua/ua/smartfon-samsung-galaxy-s22-8-256gb-phantom-white-sm-s901bzwgsek.html</x:t>
+  </x:si>
+  <x:si>
     <x:t>Смартфон Samsung Galaxy S22 8/256Gb Light Violet (SM-S901BLVGSEK)</x:t>
   </x:si>
   <x:si>
     <x:t>https://comfy.ua/ua/smartfon-samsung-galaxy-s22-8-256gb-light-violet-sm-s901blvgsek.html</x:t>
   </x:si>
   <x:si>
-    <x:t>Смартфон Samsung Galaxy S22 8/256Gb Green (SM-S901BZGGSEK)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://comfy.ua/ua/smartfon-samsung-galaxy-s22-8-256gb-green-sm-s901bzggsek.html</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Смартфон Samsung Galaxy S22 8/256Gb Phantom White (SM-S901BZWGSEK)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://comfy.ua/ua/smartfon-samsung-galaxy-s22-8-256gb-phantom-white-sm-s901bzwgsek.html</x:t>
-  </x:si>
-  <x:si>
     <x:t>Смартфон Samsung Galaxy S22+ 8/128Gb Pink (SM-S906BIDDSEK)</x:t>
   </x:si>
   <x:si>
@@ -685,12 +679,6 @@
     <x:t>https://comfy.ua/ua/smartfon-samsung-galaxy-s22-ultra-8-128gb-green-sm-s908bzgdsek.html</x:t>
   </x:si>
   <x:si>
-    <x:t>Смартфон Samsung Galaxy S22 Ultra 8/128Gb Phantom Black (SM-S908BZKDSEK)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://comfy.ua/ua/smartfon-samsung-galaxy-s22-ultra-8-128gb-phantom-black-sm-s908bzkdsek.html</x:t>
-  </x:si>
-  <x:si>
     <x:t>Смартфон Samsung Galaxy S22 Ultra 8/128Gb Phantom White (SM-S908BZWDSEK)</x:t>
   </x:si>
   <x:si>
@@ -709,16 +697,16 @@
     <x:t>https://comfy.ua/ua/smartfon-samsung-galaxy-s22-ultra-12-256gb-green-sm-s908bzggsek.html</x:t>
   </x:si>
   <x:si>
+    <x:t>Смартфон Samsung Galaxy S22 Ultra 12/256Gb Phantom White (SM-S908BZWGSEK)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://comfy.ua/ua/smartfon-samsung-galaxy-s22-ultra-12-256gb-phantom-white-sm-s908bzwgsek.html</x:t>
+  </x:si>
+  <x:si>
     <x:t>Смартфон Samsung Galaxy S22 Ultra 12/256Gb Phantom Black (SM-S908BZKGSEK)</x:t>
   </x:si>
   <x:si>
     <x:t>https://comfy.ua/ua/smartfon-samsung-galaxy-s22-ultra-12-256gb-phantom-black-sm-s908bzkgsek.html</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Смартфон Samsung Galaxy S22 Ultra 12/256Gb Phantom White (SM-S908BZWGSEK)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://comfy.ua/ua/smartfon-samsung-galaxy-s22-ultra-12-256gb-phantom-white-sm-s908bzwgsek.html</x:t>
   </x:si>
   <x:si>
     <x:t>Смартфон Samsung Galaxy S22 Ultra 12/512Gb Phantom Black (SM-S908BZKHSEK)</x:t>
@@ -2207,7 +2195,7 @@
         <x:v>201</x:v>
       </x:c>
       <x:c r="B101" s="0" t="n">
-        <x:v>35799</x:v>
+        <x:v>39399</x:v>
       </x:c>
       <x:c r="C101" s="0" t="s">
         <x:v>202</x:v>
@@ -2240,7 +2228,7 @@
         <x:v>207</x:v>
       </x:c>
       <x:c r="B104" s="0" t="n">
-        <x:v>39399</x:v>
+        <x:v>39999</x:v>
       </x:c>
       <x:c r="C104" s="0" t="s">
         <x:v>208</x:v>
@@ -2262,7 +2250,7 @@
         <x:v>211</x:v>
       </x:c>
       <x:c r="B106" s="0" t="n">
-        <x:v>39999</x:v>
+        <x:v>41999</x:v>
       </x:c>
       <x:c r="C106" s="0" t="s">
         <x:v>212</x:v>
@@ -2295,7 +2283,7 @@
         <x:v>217</x:v>
       </x:c>
       <x:c r="B109" s="0" t="n">
-        <x:v>41999</x:v>
+        <x:v>47699</x:v>
       </x:c>
       <x:c r="C109" s="0" t="s">
         <x:v>218</x:v>
@@ -2328,7 +2316,7 @@
         <x:v>223</x:v>
       </x:c>
       <x:c r="B112" s="0" t="n">
-        <x:v>47699</x:v>
+        <x:v>50299</x:v>
       </x:c>
       <x:c r="C112" s="0" t="s">
         <x:v>224</x:v>
@@ -2339,7 +2327,7 @@
         <x:v>225</x:v>
       </x:c>
       <x:c r="B113" s="0" t="n">
-        <x:v>47699</x:v>
+        <x:v>50299</x:v>
       </x:c>
       <x:c r="C113" s="0" t="s">
         <x:v>226</x:v>
@@ -2372,7 +2360,7 @@
         <x:v>231</x:v>
       </x:c>
       <x:c r="B116" s="0" t="n">
-        <x:v>50299</x:v>
+        <x:v>54999</x:v>
       </x:c>
       <x:c r="C116" s="0" t="s">
         <x:v>232</x:v>
@@ -2383,7 +2371,7 @@
         <x:v>233</x:v>
       </x:c>
       <x:c r="B117" s="0" t="n">
-        <x:v>50299</x:v>
+        <x:v>54999</x:v>
       </x:c>
       <x:c r="C117" s="0" t="s">
         <x:v>234</x:v>
@@ -2394,7 +2382,7 @@
         <x:v>235</x:v>
       </x:c>
       <x:c r="B118" s="0" t="n">
-        <x:v>54999</x:v>
+        <x:v>68999</x:v>
       </x:c>
       <x:c r="C118" s="0" t="s">
         <x:v>236</x:v>
@@ -2405,40 +2393,28 @@
         <x:v>237</x:v>
       </x:c>
       <x:c r="B119" s="0" t="n">
-        <x:v>54999</x:v>
-      </x:c>
-      <x:c r="C119" s="0" t="s">
-        <x:v>238</x:v>
+        <x:v>73999</x:v>
       </x:c>
     </x:row>
     <x:row r="120" spans="1:3">
       <x:c r="A120" s="0" t="s">
+        <x:v>238</x:v>
+      </x:c>
+      <x:c r="B120" s="0" t="n">
+        <x:v>73999</x:v>
+      </x:c>
+      <x:c r="C120" s="0" t="s">
         <x:v>239</x:v>
       </x:c>
-      <x:c r="B120" s="0" t="n">
-        <x:v>68999</x:v>
-      </x:c>
-      <x:c r="C120" s="0" t="s">
-        <x:v>240</x:v>
-      </x:c>
     </x:row>
     <x:row r="121" spans="1:3">
-      <x:c r="A121" s="0" t="s">
-        <x:v>241</x:v>
-      </x:c>
       <x:c r="B121" s="0" t="n">
-        <x:v>73999</x:v>
+        <x:v>4299</x:v>
       </x:c>
     </x:row>
     <x:row r="122" spans="1:3">
-      <x:c r="A122" s="0" t="s">
-        <x:v>242</x:v>
-      </x:c>
       <x:c r="B122" s="0" t="n">
-        <x:v>73999</x:v>
-      </x:c>
-      <x:c r="C122" s="0" t="s">
-        <x:v>243</x:v>
+        <x:v>4299</x:v>
       </x:c>
     </x:row>
     <x:row r="123" spans="1:3">
@@ -2448,17 +2424,17 @@
     </x:row>
     <x:row r="124" spans="1:3">
       <x:c r="B124" s="0" t="n">
-        <x:v>4299</x:v>
+        <x:v>4399</x:v>
       </x:c>
     </x:row>
     <x:row r="125" spans="1:3">
       <x:c r="B125" s="0" t="n">
-        <x:v>4299</x:v>
+        <x:v>4999</x:v>
       </x:c>
     </x:row>
     <x:row r="126" spans="1:3">
       <x:c r="B126" s="0" t="n">
-        <x:v>4399</x:v>
+        <x:v>4999</x:v>
       </x:c>
     </x:row>
     <x:row r="127" spans="1:3">
@@ -2473,62 +2449,62 @@
     </x:row>
     <x:row r="129" spans="1:3">
       <x:c r="B129" s="0" t="n">
-        <x:v>4999</x:v>
+        <x:v>9599</x:v>
       </x:c>
     </x:row>
     <x:row r="130" spans="1:3">
       <x:c r="B130" s="0" t="n">
-        <x:v>4999</x:v>
+        <x:v>11999</x:v>
       </x:c>
     </x:row>
     <x:row r="131" spans="1:3">
       <x:c r="B131" s="0" t="n">
-        <x:v>9599</x:v>
+        <x:v>11999</x:v>
       </x:c>
     </x:row>
     <x:row r="132" spans="1:3">
       <x:c r="B132" s="0" t="n">
-        <x:v>11999</x:v>
+        <x:v>18999</x:v>
       </x:c>
     </x:row>
     <x:row r="133" spans="1:3">
       <x:c r="B133" s="0" t="n">
-        <x:v>11999</x:v>
+        <x:v>28999</x:v>
       </x:c>
     </x:row>
     <x:row r="134" spans="1:3">
       <x:c r="B134" s="0" t="n">
-        <x:v>18999</x:v>
+        <x:v>31999</x:v>
       </x:c>
     </x:row>
     <x:row r="135" spans="1:3">
       <x:c r="B135" s="0" t="n">
-        <x:v>28999</x:v>
+        <x:v>35799</x:v>
       </x:c>
     </x:row>
     <x:row r="136" spans="1:3">
       <x:c r="B136" s="0" t="n">
-        <x:v>31999</x:v>
+        <x:v>36999</x:v>
       </x:c>
     </x:row>
     <x:row r="137" spans="1:3">
       <x:c r="B137" s="0" t="n">
-        <x:v>36999</x:v>
+        <x:v>39399</x:v>
       </x:c>
     </x:row>
     <x:row r="138" spans="1:3">
       <x:c r="B138" s="0" t="n">
-        <x:v>39399</x:v>
+        <x:v>41999</x:v>
       </x:c>
     </x:row>
     <x:row r="139" spans="1:3">
       <x:c r="B139" s="0" t="n">
-        <x:v>41999</x:v>
+        <x:v>43990</x:v>
       </x:c>
     </x:row>
     <x:row r="140" spans="1:3">
       <x:c r="B140" s="0" t="n">
-        <x:v>43990</x:v>
+        <x:v>45999</x:v>
       </x:c>
     </x:row>
     <x:row r="141" spans="1:3">
@@ -2538,7 +2514,7 @@
     </x:row>
     <x:row r="142" spans="1:3">
       <x:c r="B142" s="0" t="n">
-        <x:v>45999</x:v>
+        <x:v>47699</x:v>
       </x:c>
     </x:row>
     <x:row r="143" spans="1:3">

</xml_diff>